<commit_message>
fixed duplicate budget spread sheets
</commit_message>
<xml_diff>
--- a/Earth - Budget Spreadsheet.xlsx
+++ b/Earth - Budget Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eltdh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRED-Surface\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F311442-43BB-44C3-AE2B-E448BBCD8685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{011C3837-C95C-4654-9C2B-C283F747EEE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{005DAC11-DA2A-4DB6-B2BA-95A56AEE4B26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" xr2:uid="{005DAC11-DA2A-4DB6-B2BA-95A56AEE4B26}"/>
   </bookViews>
   <sheets>
     <sheet name="Earth - Budget" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -140,6 +142,24 @@
   </si>
   <si>
     <t>J.Salter</t>
+  </si>
+  <si>
+    <t>3D printing &amp; Laser Cutting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F.Holmes </t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Tri Track and Sorting Rig</t>
+  </si>
+  <si>
+    <t>Kinect</t>
+  </si>
+  <si>
+    <t>Tri Track</t>
   </si>
 </sst>
 </file>
@@ -149,7 +169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +228,24 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -245,7 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -260,7 +298,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -269,6 +306,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -586,29 +630,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911DD1B3-10E1-4A21-A64B-2F582D9CA3BC}">
   <dimension ref="A2:Q95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.453125" customWidth="1"/>
+    <col min="12" max="12" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B3" s="12">
         <v>43803</v>
       </c>
@@ -693,18 +737,18 @@
       </c>
       <c r="N3" s="8">
         <f>MAX(J:J)</f>
-        <v>294.66000000000003</v>
+        <v>334.66</v>
       </c>
       <c r="O3" s="8">
         <f>Q3-N3</f>
-        <v>205.33999999999997</v>
+        <v>165.33999999999997</v>
       </c>
       <c r="P3" s="9"/>
       <c r="Q3" s="8">
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B4" s="12">
         <v>43803</v>
       </c>
@@ -742,7 +786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B5" s="12">
         <v>43803</v>
       </c>
@@ -786,7 +830,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B6" s="12">
         <v>43803</v>
       </c>
@@ -832,7 +876,7 @@
         <v>454.55</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B7" s="12"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
@@ -864,7 +908,7 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
-    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B8" s="12">
         <v>43502</v>
       </c>
@@ -900,7 +944,7 @@
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
     </row>
-    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B9" s="12">
         <v>43502</v>
       </c>
@@ -936,74 +980,118 @@
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B10" s="22">
+        <v>43537</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="25">
+        <v>20</v>
+      </c>
+      <c r="G10" s="26">
+        <v>1</v>
+      </c>
+      <c r="H10" s="25">
+        <f>F10</f>
+        <v>20</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="28">
+        <f t="shared" si="1"/>
+        <v>314.66000000000003</v>
+      </c>
+      <c r="K10" s="28"/>
+      <c r="L10" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B11" s="22">
+        <v>43538</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="25">
+        <v>20</v>
+      </c>
+      <c r="G11" s="26">
+        <v>1</v>
+      </c>
+      <c r="H11" s="25">
+        <f>F11</f>
+        <v>20</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="28">
+        <f t="shared" si="1"/>
+        <v>334.66</v>
+      </c>
+      <c r="K11" s="28"/>
+      <c r="L11" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="19"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="24"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="19"/>
       <c r="B13" s="13"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="15"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="20"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B14" s="13"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="18"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="17"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="15"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K14" s="18"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B15" s="12"/>
       <c r="F15" s="6"/>
       <c r="H15" s="6" t="str">
@@ -1014,9 +1102,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K15" s="19"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B16" s="12"/>
       <c r="F16" s="6"/>
       <c r="H16" s="6" t="str">
@@ -1027,9 +1115,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" s="12"/>
       <c r="F17" s="6"/>
       <c r="H17" s="6" t="str">
@@ -1040,9 +1128,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K17" s="19"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" s="12"/>
       <c r="F18" s="6"/>
       <c r="H18" s="6" t="str">
@@ -1053,9 +1141,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K18" s="19"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" s="12"/>
       <c r="F19" s="6"/>
       <c r="H19" s="6" t="str">
@@ -1066,9 +1154,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K19" s="19"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" s="12"/>
       <c r="F20" s="6"/>
       <c r="H20" s="6" t="str">
@@ -1079,9 +1167,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K20" s="19"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21" s="12"/>
       <c r="F21" s="6"/>
       <c r="H21" s="6" t="str">
@@ -1092,9 +1180,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K21" s="19"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B22" s="12"/>
       <c r="F22" s="6"/>
       <c r="H22" s="6" t="str">
@@ -1105,9 +1193,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K22" s="19"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="18"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B23" s="12"/>
       <c r="F23" s="6"/>
       <c r="H23" s="6" t="str">
@@ -1118,9 +1206,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K23" s="19"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="18"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="F24" s="6"/>
@@ -1132,9 +1220,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K24" s="19"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="18"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B25" s="12"/>
       <c r="F25" s="6"/>
       <c r="H25" s="6" t="str">
@@ -1145,9 +1233,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K25" s="19"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="18"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B26" s="12"/>
       <c r="F26" s="6"/>
       <c r="H26" s="6" t="str">
@@ -1158,9 +1246,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K26" s="19"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="18"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B27" s="12"/>
       <c r="F27" s="6"/>
       <c r="H27" s="6" t="str">
@@ -1171,9 +1259,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K27" s="19"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="18"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B28" s="12"/>
       <c r="F28" s="6"/>
       <c r="H28" s="6" t="str">
@@ -1184,9 +1272,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K28" s="19"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="18"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B29" s="12"/>
       <c r="F29" s="6"/>
       <c r="H29" s="6" t="str">
@@ -1197,9 +1285,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K29" s="19"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="18"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B30" s="12"/>
       <c r="F30" s="6"/>
       <c r="H30" s="6" t="str">
@@ -1210,9 +1298,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K30" s="19"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="18"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B31" s="12"/>
       <c r="F31" s="6"/>
       <c r="H31" s="6" t="str">
@@ -1223,9 +1311,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K31" s="19"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="18"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B32" s="12"/>
       <c r="F32" s="6"/>
       <c r="H32" s="6" t="str">
@@ -1236,9 +1324,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K32" s="19"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="18"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B33" s="12"/>
       <c r="F33" s="6"/>
       <c r="H33" s="6" t="str">
@@ -1249,9 +1337,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K33" s="19"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="18"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B34" s="12"/>
       <c r="F34" s="6"/>
       <c r="H34" s="6" t="str">
@@ -1262,9 +1350,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K34" s="19"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="18"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B35" s="12"/>
       <c r="F35" s="6"/>
       <c r="H35" s="6" t="str">
@@ -1275,9 +1363,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K35" s="19"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="18"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B36" s="12"/>
       <c r="F36" s="6"/>
       <c r="H36" s="6" t="str">
@@ -1288,9 +1376,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K36" s="19"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="18"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B37" s="12"/>
       <c r="F37" s="6"/>
       <c r="H37" s="6" t="str">
@@ -1301,9 +1389,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K37" s="19"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="18"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B38" s="12"/>
       <c r="F38" s="6"/>
       <c r="H38" s="6" t="str">
@@ -1314,9 +1402,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K38" s="19"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="18"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B39" s="12"/>
       <c r="F39" s="6"/>
       <c r="H39" s="6" t="str">
@@ -1327,9 +1415,9 @@
         <f t="shared" ref="J39:J70" si="3">IF(G39=0,"",IF(I39="Received",J38+H39,J38))</f>
         <v/>
       </c>
-      <c r="K39" s="19"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="18"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B40" s="12"/>
       <c r="F40" s="6"/>
       <c r="H40" s="6" t="str">
@@ -1340,9 +1428,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="K40" s="19"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="18"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B41" s="12"/>
       <c r="F41" s="6"/>
       <c r="H41" s="6" t="str">
@@ -1358,7 +1446,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B42" s="12"/>
       <c r="F42" s="6"/>
       <c r="H42" s="6" t="str">
@@ -1374,7 +1462,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B43" s="12"/>
       <c r="F43" s="6"/>
       <c r="H43" s="6" t="str">
@@ -1390,7 +1478,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B44" s="12"/>
       <c r="F44" s="6"/>
       <c r="H44" s="6" t="str">
@@ -1406,7 +1494,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B45" s="12"/>
       <c r="F45" s="6"/>
       <c r="H45" s="6" t="str">
@@ -1422,7 +1510,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B46" s="12"/>
       <c r="F46" s="6"/>
       <c r="H46" s="6" t="str">
@@ -1438,7 +1526,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B47" s="12"/>
       <c r="F47" s="6"/>
       <c r="H47" s="6" t="str">
@@ -1454,7 +1542,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B48" s="12"/>
       <c r="F48" s="6"/>
       <c r="H48" s="6" t="str">
@@ -1470,7 +1558,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B49" s="12"/>
       <c r="F49" s="6"/>
       <c r="H49" s="6" t="str">
@@ -1486,7 +1574,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B50" s="12"/>
       <c r="F50" s="6"/>
       <c r="H50" s="6" t="str">
@@ -1502,7 +1590,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B51" s="12"/>
       <c r="F51" s="6"/>
       <c r="H51" s="6" t="str">
@@ -1518,7 +1606,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B52" s="12"/>
       <c r="F52" s="6"/>
       <c r="H52" s="6" t="str">
@@ -1534,7 +1622,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B53" s="12"/>
       <c r="F53" s="6"/>
       <c r="H53" s="6" t="str">
@@ -1550,7 +1638,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B54" s="12"/>
       <c r="F54" s="6"/>
       <c r="H54" s="6" t="str">
@@ -1566,7 +1654,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B55" s="12"/>
       <c r="F55" s="6"/>
       <c r="H55" s="6" t="str">
@@ -1582,7 +1670,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B56" s="12"/>
       <c r="F56" s="6"/>
       <c r="H56" s="6" t="str">
@@ -1598,7 +1686,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B57" s="12"/>
       <c r="F57" s="6"/>
       <c r="H57" s="6" t="str">
@@ -1614,7 +1702,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B58" s="12"/>
       <c r="F58" s="6"/>
       <c r="H58" s="6" t="str">
@@ -1630,7 +1718,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B59" s="12"/>
       <c r="F59" s="6"/>
       <c r="J59" s="5" t="str">
@@ -1642,7 +1730,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B60" s="12"/>
       <c r="F60" s="6"/>
       <c r="J60" s="5" t="str">
@@ -1654,7 +1742,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B61" s="12"/>
       <c r="F61" s="6"/>
       <c r="J61" s="5" t="str">
@@ -1666,7 +1754,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B62" s="12"/>
       <c r="F62" s="6"/>
       <c r="J62" s="5" t="str">
@@ -1678,7 +1766,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B63" s="12"/>
       <c r="F63" s="6"/>
       <c r="J63" s="5" t="str">
@@ -1690,7 +1778,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B64" s="12"/>
       <c r="F64" s="6"/>
       <c r="J64" s="5" t="str">
@@ -1702,7 +1790,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B65" s="12"/>
       <c r="F65" s="6"/>
       <c r="J65" s="5" t="str">
@@ -1714,7 +1802,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B66" s="12"/>
       <c r="F66" s="6"/>
       <c r="J66" s="5" t="str">
@@ -1726,7 +1814,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F67" s="6"/>
       <c r="J67" s="5" t="str">
         <f t="shared" si="3"/>
@@ -1737,7 +1825,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F68" s="6"/>
       <c r="J68" s="5" t="str">
         <f t="shared" si="3"/>
@@ -1748,7 +1836,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F69" s="6"/>
       <c r="J69" s="5" t="str">
         <f t="shared" si="3"/>
@@ -1759,7 +1847,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F70" s="6"/>
       <c r="J70" s="5" t="str">
         <f t="shared" si="3"/>
@@ -1770,7 +1858,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F71" s="6"/>
       <c r="J71" s="5" t="str">
         <f t="shared" ref="J71:J94" si="5">IF(G71=0,"",IF(I71="Received",J70+H71,J70))</f>
@@ -1781,7 +1869,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F72" s="6"/>
       <c r="J72" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1792,7 +1880,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F73" s="6"/>
       <c r="J73" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1803,7 +1891,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F74" s="6"/>
       <c r="J74" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1814,7 +1902,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F75" s="6"/>
       <c r="J75" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1825,7 +1913,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F76" s="6"/>
       <c r="J76" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1836,7 +1924,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F77" s="6"/>
       <c r="J77" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1847,7 +1935,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F78" s="6"/>
       <c r="J78" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1858,7 +1946,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F79" s="6"/>
       <c r="J79" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1869,7 +1957,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F80" s="6"/>
       <c r="J80" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1880,7 +1968,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F81" s="6"/>
       <c r="J81" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1891,7 +1979,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F82" s="6"/>
       <c r="J82" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1902,7 +1990,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F83" s="6"/>
       <c r="J83" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1913,7 +2001,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F84" s="6"/>
       <c r="J84" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1924,7 +2012,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F85" s="6"/>
       <c r="J85" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1935,7 +2023,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F86" s="6"/>
       <c r="J86" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1946,7 +2034,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F87" s="6"/>
       <c r="J87" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1957,7 +2045,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F88" s="6"/>
       <c r="J88" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1968,7 +2056,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F89" s="6"/>
       <c r="J89" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1979,7 +2067,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F90" s="6"/>
       <c r="J90" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1990,7 +2078,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F91" s="6"/>
       <c r="J91" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2001,7 +2089,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F92" s="6"/>
       <c r="J92" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2012,7 +2100,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F93" s="6"/>
       <c r="J93" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2023,7 +2111,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F94" s="6"/>
       <c r="J94" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2034,7 +2122,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:11" x14ac:dyDescent="0.35">
       <c r="K95" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>

</xml_diff>

<commit_message>
tidying up readme and budget
</commit_message>
<xml_diff>
--- a/Earth - Budget Spreadsheet.xlsx
+++ b/Earth - Budget Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRED-Surface\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\E-ProjectDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{011C3837-C95C-4654-9C2B-C283F747EEE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2381A932-4853-4433-9EF5-042016B63AA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" xr2:uid="{005DAC11-DA2A-4DB6-B2BA-95A56AEE4B26}"/>
+    <workbookView xWindow="1530" yWindow="5025" windowWidth="28290" windowHeight="13020" xr2:uid="{005DAC11-DA2A-4DB6-B2BA-95A56AEE4B26}"/>
   </bookViews>
   <sheets>
     <sheet name="Earth - Budget" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -52,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -121,12 +119,6 @@
   </si>
   <si>
     <t>DC Power Jack</t>
-  </si>
-  <si>
-    <t>Estimated Spending</t>
-  </si>
-  <si>
-    <t>Estimated Budget Remaing</t>
   </si>
   <si>
     <t>Cumulative Estimated Budget</t>
@@ -247,18 +239,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -283,7 +269,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -303,7 +289,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -313,6 +298,8 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -630,29 +617,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911DD1B3-10E1-4A21-A64B-2F582D9CA3BC}">
   <dimension ref="A2:Q95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.453125" customWidth="1"/>
-    <col min="12" max="12" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +669,7 @@
         <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>9</v>
@@ -698,7 +686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="12">
         <v>43803</v>
       </c>
@@ -748,7 +736,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="12">
         <v>43803</v>
       </c>
@@ -786,7 +774,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>43803</v>
       </c>
@@ -823,14 +811,10 @@
       <c r="L5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+    </row>
+    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="12">
         <v>43803</v>
       </c>
@@ -867,23 +851,17 @@
       <c r="L6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="8">
-        <f>MAX(K:K)</f>
-        <v>45.45</v>
-      </c>
-      <c r="O6" s="8">
-        <f>Q3-N6</f>
-        <v>454.55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+    </row>
+    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="6">
         <v>18.27</v>
@@ -908,18 +886,18 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
-    <row r="8" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="12">
         <v>43502</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F8" s="6">
         <v>216.58</v>
@@ -939,23 +917,23 @@
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
     </row>
-    <row r="9" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>43502</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F9" s="6">
         <v>14.36</v>
@@ -975,99 +953,99 @@
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B10" s="22">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="21">
         <v>43537</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="25">
+      <c r="E10" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="24">
         <v>20</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="25">
         <v>1</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="24">
         <f>F10</f>
         <v>20</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="27">
         <f t="shared" si="1"/>
         <v>314.66000000000003</v>
       </c>
-      <c r="K10" s="28"/>
-      <c r="L10" s="24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B11" s="22">
+      <c r="K10" s="27"/>
+      <c r="L10" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="21">
         <v>43538</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="25">
+      <c r="D11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="24">
         <v>20</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="25">
         <v>1</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="24">
         <f>F11</f>
         <v>20</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="27">
         <f t="shared" si="1"/>
         <v>334.66</v>
       </c>
-      <c r="K11" s="28"/>
-      <c r="L11" s="24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="19"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="24"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="19"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="23"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
       <c r="B13" s="13"/>
-      <c r="C13" s="20"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
@@ -1078,9 +1056,9 @@
       <c r="K13" s="18"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
-      <c r="C14" s="21"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
@@ -1091,7 +1069,7 @@
       <c r="K14" s="18"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="F15" s="6"/>
       <c r="H15" s="6" t="str">
@@ -1104,7 +1082,7 @@
       </c>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="12"/>
       <c r="F16" s="6"/>
       <c r="H16" s="6" t="str">
@@ -1117,7 +1095,7 @@
       </c>
       <c r="K16" s="18"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="F17" s="6"/>
       <c r="H17" s="6" t="str">
@@ -1130,7 +1108,7 @@
       </c>
       <c r="K17" s="18"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="F18" s="6"/>
       <c r="H18" s="6" t="str">
@@ -1143,7 +1121,7 @@
       </c>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="F19" s="6"/>
       <c r="H19" s="6" t="str">
@@ -1156,7 +1134,7 @@
       </c>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
       <c r="F20" s="6"/>
       <c r="H20" s="6" t="str">
@@ -1169,7 +1147,7 @@
       </c>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="12"/>
       <c r="F21" s="6"/>
       <c r="H21" s="6" t="str">
@@ -1182,7 +1160,7 @@
       </c>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="F22" s="6"/>
       <c r="H22" s="6" t="str">
@@ -1195,7 +1173,7 @@
       </c>
       <c r="K22" s="18"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
       <c r="F23" s="6"/>
       <c r="H23" s="6" t="str">
@@ -1208,7 +1186,7 @@
       </c>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="F24" s="6"/>
@@ -1222,7 +1200,7 @@
       </c>
       <c r="K24" s="18"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="12"/>
       <c r="F25" s="6"/>
       <c r="H25" s="6" t="str">
@@ -1235,7 +1213,7 @@
       </c>
       <c r="K25" s="18"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="12"/>
       <c r="F26" s="6"/>
       <c r="H26" s="6" t="str">
@@ -1248,7 +1226,7 @@
       </c>
       <c r="K26" s="18"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="F27" s="6"/>
       <c r="H27" s="6" t="str">
@@ -1261,7 +1239,7 @@
       </c>
       <c r="K27" s="18"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
       <c r="F28" s="6"/>
       <c r="H28" s="6" t="str">
@@ -1274,7 +1252,7 @@
       </c>
       <c r="K28" s="18"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="F29" s="6"/>
       <c r="H29" s="6" t="str">
@@ -1287,7 +1265,7 @@
       </c>
       <c r="K29" s="18"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="12"/>
       <c r="F30" s="6"/>
       <c r="H30" s="6" t="str">
@@ -1300,7 +1278,7 @@
       </c>
       <c r="K30" s="18"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="F31" s="6"/>
       <c r="H31" s="6" t="str">
@@ -1313,7 +1291,7 @@
       </c>
       <c r="K31" s="18"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
       <c r="F32" s="6"/>
       <c r="H32" s="6" t="str">
@@ -1326,7 +1304,7 @@
       </c>
       <c r="K32" s="18"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
       <c r="F33" s="6"/>
       <c r="H33" s="6" t="str">
@@ -1339,7 +1317,7 @@
       </c>
       <c r="K33" s="18"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
       <c r="F34" s="6"/>
       <c r="H34" s="6" t="str">
@@ -1352,7 +1330,7 @@
       </c>
       <c r="K34" s="18"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
       <c r="F35" s="6"/>
       <c r="H35" s="6" t="str">
@@ -1365,7 +1343,7 @@
       </c>
       <c r="K35" s="18"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="12"/>
       <c r="F36" s="6"/>
       <c r="H36" s="6" t="str">
@@ -1378,7 +1356,7 @@
       </c>
       <c r="K36" s="18"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
       <c r="F37" s="6"/>
       <c r="H37" s="6" t="str">
@@ -1391,7 +1369,7 @@
       </c>
       <c r="K37" s="18"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="12"/>
       <c r="F38" s="6"/>
       <c r="H38" s="6" t="str">
@@ -1404,7 +1382,7 @@
       </c>
       <c r="K38" s="18"/>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="12"/>
       <c r="F39" s="6"/>
       <c r="H39" s="6" t="str">
@@ -1417,7 +1395,7 @@
       </c>
       <c r="K39" s="18"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
       <c r="F40" s="6"/>
       <c r="H40" s="6" t="str">
@@ -1430,7 +1408,7 @@
       </c>
       <c r="K40" s="18"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="12"/>
       <c r="F41" s="6"/>
       <c r="H41" s="6" t="str">
@@ -1446,7 +1424,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
       <c r="F42" s="6"/>
       <c r="H42" s="6" t="str">
@@ -1462,7 +1440,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="12"/>
       <c r="F43" s="6"/>
       <c r="H43" s="6" t="str">
@@ -1478,7 +1456,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
       <c r="F44" s="6"/>
       <c r="H44" s="6" t="str">
@@ -1494,7 +1472,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="12"/>
       <c r="F45" s="6"/>
       <c r="H45" s="6" t="str">
@@ -1510,7 +1488,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
       <c r="F46" s="6"/>
       <c r="H46" s="6" t="str">
@@ -1526,7 +1504,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="F47" s="6"/>
       <c r="H47" s="6" t="str">
@@ -1542,7 +1520,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
       <c r="F48" s="6"/>
       <c r="H48" s="6" t="str">
@@ -1558,7 +1536,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="F49" s="6"/>
       <c r="H49" s="6" t="str">
@@ -1574,7 +1552,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
       <c r="F50" s="6"/>
       <c r="H50" s="6" t="str">
@@ -1590,7 +1568,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="12"/>
       <c r="F51" s="6"/>
       <c r="H51" s="6" t="str">
@@ -1606,7 +1584,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="12"/>
       <c r="F52" s="6"/>
       <c r="H52" s="6" t="str">
@@ -1622,7 +1600,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="12"/>
       <c r="F53" s="6"/>
       <c r="H53" s="6" t="str">
@@ -1638,7 +1616,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="12"/>
       <c r="F54" s="6"/>
       <c r="H54" s="6" t="str">
@@ -1654,7 +1632,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="12"/>
       <c r="F55" s="6"/>
       <c r="H55" s="6" t="str">
@@ -1670,7 +1648,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="12"/>
       <c r="F56" s="6"/>
       <c r="H56" s="6" t="str">
@@ -1686,7 +1664,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" s="12"/>
       <c r="F57" s="6"/>
       <c r="H57" s="6" t="str">
@@ -1702,7 +1680,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="F58" s="6"/>
       <c r="H58" s="6" t="str">
@@ -1718,7 +1696,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" s="12"/>
       <c r="F59" s="6"/>
       <c r="J59" s="5" t="str">
@@ -1730,7 +1708,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="12"/>
       <c r="F60" s="6"/>
       <c r="J60" s="5" t="str">
@@ -1742,7 +1720,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="12"/>
       <c r="F61" s="6"/>
       <c r="J61" s="5" t="str">
@@ -1754,7 +1732,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="12"/>
       <c r="F62" s="6"/>
       <c r="J62" s="5" t="str">
@@ -1766,7 +1744,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" s="12"/>
       <c r="F63" s="6"/>
       <c r="J63" s="5" t="str">
@@ -1778,7 +1756,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="12"/>
       <c r="F64" s="6"/>
       <c r="J64" s="5" t="str">
@@ -1790,7 +1768,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="12"/>
       <c r="F65" s="6"/>
       <c r="J65" s="5" t="str">
@@ -1802,7 +1780,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" s="12"/>
       <c r="F66" s="6"/>
       <c r="J66" s="5" t="str">
@@ -1814,7 +1792,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F67" s="6"/>
       <c r="J67" s="5" t="str">
         <f t="shared" si="3"/>
@@ -1825,7 +1803,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F68" s="6"/>
       <c r="J68" s="5" t="str">
         <f t="shared" si="3"/>
@@ -1836,7 +1814,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F69" s="6"/>
       <c r="J69" s="5" t="str">
         <f t="shared" si="3"/>
@@ -1847,7 +1825,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F70" s="6"/>
       <c r="J70" s="5" t="str">
         <f t="shared" si="3"/>
@@ -1858,7 +1836,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F71" s="6"/>
       <c r="J71" s="5" t="str">
         <f t="shared" ref="J71:J94" si="5">IF(G71=0,"",IF(I71="Received",J70+H71,J70))</f>
@@ -1869,7 +1847,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F72" s="6"/>
       <c r="J72" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1880,7 +1858,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F73" s="6"/>
       <c r="J73" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1891,7 +1869,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F74" s="6"/>
       <c r="J74" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1902,7 +1880,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F75" s="6"/>
       <c r="J75" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1913,7 +1891,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F76" s="6"/>
       <c r="J76" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1924,7 +1902,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F77" s="6"/>
       <c r="J77" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1935,7 +1913,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F78" s="6"/>
       <c r="J78" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1946,7 +1924,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F79" s="6"/>
       <c r="J79" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1957,7 +1935,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F80" s="6"/>
       <c r="J80" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1968,7 +1946,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F81" s="6"/>
       <c r="J81" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1979,7 +1957,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F82" s="6"/>
       <c r="J82" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1990,7 +1968,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F83" s="6"/>
       <c r="J83" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2001,7 +1979,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F84" s="6"/>
       <c r="J84" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2012,7 +1990,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F85" s="6"/>
       <c r="J85" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2023,7 +2001,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F86" s="6"/>
       <c r="J86" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2034,7 +2012,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F87" s="6"/>
       <c r="J87" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2045,7 +2023,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F88" s="6"/>
       <c r="J88" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2056,7 +2034,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F89" s="6"/>
       <c r="J89" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2067,7 +2045,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F90" s="6"/>
       <c r="J90" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2078,7 +2056,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F91" s="6"/>
       <c r="J91" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2089,7 +2067,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F92" s="6"/>
       <c r="J92" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2100,7 +2078,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F93" s="6"/>
       <c r="J93" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2111,7 +2089,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F94" s="6"/>
       <c r="J94" s="5" t="str">
         <f t="shared" si="5"/>
@@ -2122,7 +2100,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="6:11" x14ac:dyDescent="0.25">
       <c r="K95" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>

</xml_diff>